<commit_message>
spelling + slight changes to the timeline
</commit_message>
<xml_diff>
--- a/timeline.xlsx
+++ b/timeline.xlsx
@@ -1,17 +1,28 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="17426"/>
-  <workbookPr filterPrivacy="1" defaultThemeVersion="164011"/>
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="27510"/>
+  <workbookPr filterPrivacy="1"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/sheyne/Documents/sinap-design-docs/"/>
+    </mc:Choice>
+  </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12645"/>
+    <workbookView xWindow="880" yWindow="460" windowWidth="22260" windowHeight="12640"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="162913"/>
+  <calcPr calcId="150001" concurrentCalc="0"/>
   <extLst>
-    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{79F54976-1DA5-4618-B147-4CDE4B953A38}">
+      <x14:workbookPr defaultImageDpi="32767"/>
+    </ext>
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{7523E5D3-25F3-A5E0-1632-64F254C22452}">
+      <mx:ArchID Flags="2"/>
+    </ext>
+    <ext uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
     </ext>
   </extLst>
@@ -19,7 +30,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="72" uniqueCount="25">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="72" uniqueCount="26">
   <si>
     <t>Week</t>
   </si>
@@ -78,12 +89,6 @@
     <t>Reverse debugging</t>
   </si>
   <si>
-    <t>Graph beutification</t>
-  </si>
-  <si>
-    <t>Graph beutification specialization</t>
-  </si>
-  <si>
     <t>Custom node images</t>
   </si>
   <si>
@@ -94,12 +99,21 @@
   </si>
   <si>
     <t>Circuit design plugin</t>
+  </si>
+  <si>
+    <t>Graph beautification</t>
+  </si>
+  <si>
+    <t>Graph beautification specialization</t>
+  </si>
+  <si>
+    <t>Plugin-interface specification</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <fonts count="1" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -449,19 +463,19 @@
   <dimension ref="A1:F17"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C32" sqref="C32"/>
+      <selection activeCell="B22" sqref="B22"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="12" customWidth="1"/>
     <col min="2" max="2" width="27.33203125" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="25.19921875" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="25.1640625" bestFit="1" customWidth="1"/>
     <col min="4" max="5" width="25.6640625" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="19.86328125" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="19.83203125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -481,12 +495,12 @@
         <v>5</v>
       </c>
     </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="2" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A2" s="1">
         <v>42744</v>
       </c>
       <c r="B2" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="C2" t="s">
         <v>11</v>
@@ -498,12 +512,12 @@
         <v>11</v>
       </c>
     </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="3" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A3" s="1">
         <v>42751</v>
       </c>
       <c r="B3" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="C3" t="s">
         <v>11</v>
@@ -515,12 +529,12 @@
         <v>11</v>
       </c>
     </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="4" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A4" s="1">
         <v>42758</v>
       </c>
       <c r="B4" t="s">
-        <v>10</v>
+        <v>25</v>
       </c>
       <c r="C4" t="s">
         <v>12</v>
@@ -532,12 +546,12 @@
         <v>12</v>
       </c>
     </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="5" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A5" s="1">
         <v>42765</v>
       </c>
       <c r="B5" t="s">
-        <v>10</v>
+        <v>25</v>
       </c>
       <c r="C5" t="s">
         <v>12</v>
@@ -549,7 +563,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="6" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A6" s="1">
         <v>42772</v>
       </c>
@@ -566,7 +580,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="7" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="7" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A7" s="1">
         <v>42779</v>
       </c>
@@ -586,12 +600,12 @@
         <v>6</v>
       </c>
     </row>
-    <row r="8" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="8" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A8" s="1">
         <v>42786</v>
       </c>
       <c r="B8" t="s">
-        <v>19</v>
+        <v>23</v>
       </c>
       <c r="C8" t="s">
         <v>15</v>
@@ -603,12 +617,12 @@
         <v>16</v>
       </c>
     </row>
-    <row r="9" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="9" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A9" s="1">
         <v>42793</v>
       </c>
       <c r="B9" t="s">
-        <v>19</v>
+        <v>23</v>
       </c>
       <c r="C9" t="s">
         <v>15</v>
@@ -620,38 +634,38 @@
         <v>16</v>
       </c>
     </row>
-    <row r="10" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="10" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A10" s="1">
         <v>42800</v>
       </c>
       <c r="B10" t="s">
-        <v>19</v>
+        <v>23</v>
       </c>
       <c r="C10" t="s">
         <v>15</v>
       </c>
       <c r="D10" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="E10" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="11" spans="1:6" x14ac:dyDescent="0.45">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="11" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A11" s="1">
         <v>42807</v>
       </c>
       <c r="B11" t="s">
-        <v>20</v>
+        <v>24</v>
       </c>
       <c r="D11" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="E11" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="12" spans="1:6" x14ac:dyDescent="0.45">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="12" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A12" s="1">
         <v>42814</v>
       </c>
@@ -671,7 +685,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="13" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="13" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A13" s="1">
         <v>42821</v>
       </c>
@@ -688,7 +702,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="14" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="14" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A14" s="1">
         <v>42828</v>
       </c>
@@ -705,55 +719,55 @@
         <v>18</v>
       </c>
     </row>
-    <row r="15" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="15" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A15" s="1">
         <v>42835</v>
       </c>
       <c r="B15" t="s">
+        <v>20</v>
+      </c>
+      <c r="C15" t="s">
+        <v>21</v>
+      </c>
+      <c r="D15" t="s">
+        <v>20</v>
+      </c>
+      <c r="E15" t="s">
         <v>22</v>
       </c>
-      <c r="C15" t="s">
-        <v>23</v>
-      </c>
-      <c r="D15" t="s">
-        <v>22</v>
-      </c>
-      <c r="E15" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="16" spans="1:6" x14ac:dyDescent="0.45">
+    </row>
+    <row r="16" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A16" s="1">
         <v>42842</v>
       </c>
       <c r="B16" t="s">
+        <v>20</v>
+      </c>
+      <c r="C16" t="s">
+        <v>21</v>
+      </c>
+      <c r="D16" t="s">
+        <v>20</v>
+      </c>
+      <c r="E16" t="s">
         <v>22</v>
       </c>
-      <c r="C16" t="s">
-        <v>23</v>
-      </c>
-      <c r="D16" t="s">
-        <v>22</v>
-      </c>
-      <c r="E16" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="17" spans="1:6" x14ac:dyDescent="0.45">
+    </row>
+    <row r="17" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A17" s="1">
         <v>42849</v>
       </c>
       <c r="B17" t="s">
+        <v>20</v>
+      </c>
+      <c r="C17" t="s">
+        <v>21</v>
+      </c>
+      <c r="D17" t="s">
+        <v>20</v>
+      </c>
+      <c r="E17" t="s">
         <v>22</v>
-      </c>
-      <c r="C17" t="s">
-        <v>23</v>
-      </c>
-      <c r="D17" t="s">
-        <v>22</v>
-      </c>
-      <c r="E17" t="s">
-        <v>24</v>
       </c>
       <c r="F17" t="s">
         <v>8</v>

</xml_diff>

<commit_message>
Added table for timeline to DD.
</commit_message>
<xml_diff>
--- a/timeline.xlsx
+++ b/timeline.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="72" uniqueCount="25">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="73" uniqueCount="26">
   <si>
     <t>Week</t>
   </si>
@@ -94,6 +94,9 @@
   </si>
   <si>
     <t>Circuit design plugin</t>
+  </si>
+  <si>
+    <t>Pushdown automata support</t>
   </si>
 </sst>
 </file>
@@ -449,7 +452,7 @@
   <dimension ref="A1:F17"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C32" sqref="C32"/>
+      <selection activeCell="C12" sqref="C12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
@@ -644,6 +647,9 @@
       <c r="B11" t="s">
         <v>20</v>
       </c>
+      <c r="C11" t="s">
+        <v>25</v>
+      </c>
       <c r="D11" t="s">
         <v>21</v>
       </c>

</xml_diff>